<commit_message>
Reanalysis with the latest data (Updated graphs)
</commit_message>
<xml_diff>
--- a/resultData/signatures_by_num_destIP(created 20220109).xlsx
+++ b/resultData/signatures_by_num_destIP(created 20220109).xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shion\PycharmProjects\ProjectRoute112021\resultData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{96939D24-9CF5-4ECF-9A22-E2306CCAC3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5A18AB-8FCC-4172-9E66-D33CCDF24086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17740"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="signatures_by_num_destIP(2021.1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="378">
   <si>
     <t>Signature</t>
   </si>
@@ -1145,12 +1145,21 @@
   </si>
   <si>
     <t>CVE</t>
+  </si>
+  <si>
+    <t>CVE-2018-14558,CVE-2020-10987</t>
+  </si>
+  <si>
+    <t>CVE-2021-26084</t>
+  </si>
+  <si>
+    <t>CVE-2014-3206</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -2002,16 +2011,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="37.90625" customWidth="1"/>
+    <col min="4" max="4" width="57.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2038,6 +2048,9 @@
       <c r="C2">
         <v>1117</v>
       </c>
+      <c r="D2" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
@@ -2049,6 +2062,9 @@
       <c r="C3">
         <v>458</v>
       </c>
+      <c r="D3" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
@@ -2060,6 +2076,9 @@
       <c r="C4">
         <v>281</v>
       </c>
+      <c r="D4" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
@@ -2192,6 +2211,9 @@
       <c r="C16">
         <v>3428</v>
       </c>
+      <c r="D16" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
@@ -6111,5 +6133,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>